<commit_message>
Actualizacion dólar Chile 2020, 2021, 2022, 2023 y 2024
</commit_message>
<xml_diff>
--- a/dolar/chile/excel/v1/cl/dolarCL_2024.xlsx
+++ b/dolar/chile/excel/v1/cl/dolarCL_2024.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B182"/>
+  <dimension ref="A1:B184"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2563,17 +2563,41 @@
         </is>
       </c>
     </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>10-09-2024</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>946,22</t>
+        </is>
+      </c>
+    </row>
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
+          <t>11-09-2024</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>948,85</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
           <t>Pie de página: Reporte generado automáticamente.</t>
         </is>
       </c>
     </row>
-    <row r="182">
-      <c r="A182" t="inlineStr">
-        <is>
-          <t>Última actualización: 2024-09-08T07:38:50Z</t>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>Última actualización: 2024-09-10T21:15:11Z</t>
         </is>
       </c>
     </row>

</xml_diff>